<commit_message>
product backlog content added
</commit_message>
<xml_diff>
--- a/product_backlog.xlsx
+++ b/product_backlog.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://htldornbirn-my.sharepoint.com/personal/damiano_pezze_student_htldornbirn_at/Documents/4bWI/Smart_City_Ecolyzer/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="76" documentId="11_AD4DB114E441178AC67DF4581650EF04683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{181930EE-3F7C-4470-A5C9-7462E25CC47D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$C$12</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -18,8 +27,59 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>Story</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Storypoints</t>
+  </si>
+  <si>
+    <t>Ich als User sehe die Anzahl an Fahrrädern am jeweiligen Standort</t>
+  </si>
+  <si>
+    <t>Ich als User sehe die Anzahl an Autos am jeweiligen Standort</t>
+  </si>
+  <si>
+    <t>Ich als User sehe die Anzahl an Fußgängern am jeweiligen Standort</t>
+  </si>
+  <si>
+    <t>Ich als User sehe die geschätzten Emissionen</t>
+  </si>
+  <si>
+    <t>Ich als User sehe eine Heat-Map (An welchem Standort ist wie viel Verkehr)</t>
+  </si>
+  <si>
+    <t>Ich als User kann eine dynamische Route zum Ziel generieren lassen (möglichst wenig Verkehr)</t>
+  </si>
+  <si>
+    <t>Ich als User habe eine Website</t>
+  </si>
+  <si>
+    <t>Ich als User habe eine App</t>
+  </si>
+  <si>
+    <t>Ich als User sehe die Anzahl an Lastwagen und Busse am jeweiligen Standort</t>
+  </si>
+  <si>
+    <t>Ich als User sehe die Eco-Quote (Quote: Umweltfreundlich / nicht Umweltfreundlich;
+Unterscheidung Auto, Lastwagen, Fahrrad)</t>
+  </si>
+  <si>
+    <t>1,2,3,5,8,13,21, 34</t>
+  </si>
+  <si>
+    <t>Ich als User kann auf einzelne Standorte klicken und Daten sehen</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,12 +89,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,11 +115,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -66,6 +136,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +404,164 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="82" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C12" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C12">
+      <sortCondition descending="1" ref="B1:B12"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G12">
+    <sortCondition descending="1" ref="A1:A12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tutorial for vehicle detection
</commit_message>
<xml_diff>
--- a/product_backlog.xlsx
+++ b/product_backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -18,10 +18,21 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$C$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -39,51 +50,51 @@
     <t>Storypoints</t>
   </si>
   <si>
+    <t>Ich als User sehe die Anzahl an Autos am jeweiligen Standort</t>
+  </si>
+  <si>
+    <t>1,2,3,5,8,13,21, 34</t>
+  </si>
+  <si>
+    <t>Ich als User habe eine Website</t>
+  </si>
+  <si>
+    <t>Ich als User sehe die Anzahl an Fußgängern am jeweiligen Standort</t>
+  </si>
+  <si>
+    <t>Ich als User sehe die Anzahl an Lastwagen und Busse am jeweiligen Standort</t>
+  </si>
+  <si>
     <t>Ich als User sehe die Anzahl an Fahrrädern am jeweiligen Standort</t>
   </si>
   <si>
-    <t>Ich als User sehe die Anzahl an Autos am jeweiligen Standort</t>
-  </si>
-  <si>
-    <t>Ich als User sehe die Anzahl an Fußgängern am jeweiligen Standort</t>
-  </si>
-  <si>
-    <t>Ich als User sehe die geschätzten Emissionen</t>
+    <t>Ich als User kann auf einzelne Standorte klicken und Daten sehen</t>
   </si>
   <si>
     <t>Ich als User sehe eine Heat-Map (An welchem Standort ist wie viel Verkehr)</t>
-  </si>
-  <si>
-    <t>Ich als User kann eine dynamische Route zum Ziel generieren lassen (möglichst wenig Verkehr)</t>
-  </si>
-  <si>
-    <t>Ich als User habe eine Website</t>
-  </si>
-  <si>
-    <t>Ich als User habe eine App</t>
-  </si>
-  <si>
-    <t>Ich als User sehe die Anzahl an Lastwagen und Busse am jeweiligen Standort</t>
   </si>
   <si>
     <t>Ich als User sehe die Eco-Quote (Quote: Umweltfreundlich / nicht Umweltfreundlich;
 Unterscheidung Auto, Lastwagen, Fahrrad)</t>
   </si>
   <si>
-    <t>1,2,3,5,8,13,21, 34</t>
-  </si>
-  <si>
-    <t>Ich als User kann auf einzelne Standorte klicken und Daten sehen</t>
-  </si>
-  <si>
     <t>Ich als User kann die Zeit per slider zurückdrehen bzw. die Entwicklung des Verkehrs sehen</t>
+  </si>
+  <si>
+    <t>Ich als User sehe die geschätzten Emissionen</t>
+  </si>
+  <si>
+    <t>Ich als User habe eine App</t>
+  </si>
+  <si>
+    <t>Ich als User kann eine dynamische Route zum Ziel generieren lassen (möglichst wenig Verkehr)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,14 +421,14 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="82" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,9 +439,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -439,12 +450,12 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -453,9 +464,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>9</v>
@@ -464,9 +475,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>9</v>
@@ -475,9 +486,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -486,9 +497,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>9</v>
@@ -497,9 +508,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>8</v>
@@ -508,9 +519,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="29.1">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -519,9 +530,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -530,9 +541,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -541,9 +552,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -552,9 +563,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>1</v>

</xml_diff>